<commit_message>
DRC Config File added
</commit_message>
<xml_diff>
--- a/Excels/DRC.xlsx
+++ b/Excels/DRC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -3386,8 +3386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,10 +3445,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2390932</v>
+        <v>2394650</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>137</v>
@@ -3740,7 +3740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>